<commit_message>
Se actualiza archivo de encuesta
</commit_message>
<xml_diff>
--- a/data/raw/survey_ready.xlsx
+++ b/data/raw/survey_ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4890E762-F3E0-4E33-A3F1-84967A96B160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610DC131-37AC-4EF7-A49F-8D93841E1F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respuestas de formulario 1'!$H$1:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respuestas de formulario 1'!$AE$1:$AE$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="255">
   <si>
     <t>Femenino</t>
   </si>
@@ -804,6 +804,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mejora de salarios principalmente, quizas alguna otra prestacion de ley. </t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -865,7 +868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1110,6 +1113,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1164,9 +1178,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1182,22 +1193,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1205,9 +1207,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1220,8 +1219,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1244,6 +1241,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1496,9 +1504,9 @@
   </sheetPr>
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG16" sqref="AG16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1534,7 @@
     <col min="21" max="21" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.44140625" customWidth="1"/>
     <col min="25" max="25" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.88671875" bestFit="1" customWidth="1"/>
@@ -1675,10 +1683,10 @@
       <c r="F2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="39" t="s">
         <v>113</v>
       </c>
       <c r="I2" s="5">
@@ -1687,7 +1695,9 @@
       <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5">
+        <v>1</v>
+      </c>
       <c r="L2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1724,8 +1734,10 @@
       <c r="W2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5" t="s">
+      <c r="X2" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="39" t="s">
         <v>6</v>
       </c>
       <c r="Z2" s="5">
@@ -1734,11 +1746,15 @@
       <c r="AA2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="5"/>
+      <c r="AB2" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="AC2" s="5">
         <v>70</v>
       </c>
-      <c r="AD2" s="5"/>
+      <c r="AD2" s="5" t="s">
+        <v>254</v>
+      </c>
       <c r="AE2" s="5">
         <v>48</v>
       </c>
@@ -1765,10 +1781,10 @@
       <c r="A3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -1780,7 +1796,7 @@
       <c r="F3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="38" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1831,8 +1847,10 @@
       <c r="W3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="8" t="s">
+      <c r="X3" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z3" s="8">
@@ -1841,7 +1859,9 @@
       <c r="AA3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="10"/>
+      <c r="AB3" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AC3" s="8">
         <v>48</v>
       </c>
@@ -1874,7 +1894,7 @@
       <c r="A4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -1889,7 +1909,7 @@
       <c r="F4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H4" s="13" t="s">
@@ -1901,7 +1921,9 @@
       <c r="J4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="15">
+        <v>1</v>
+      </c>
       <c r="L4" s="13" t="s">
         <v>12</v>
       </c>
@@ -1938,8 +1960,10 @@
       <c r="W4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="13" t="s">
+      <c r="X4" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z4" s="13">
@@ -1954,7 +1978,9 @@
       <c r="AC4" s="13">
         <v>29</v>
       </c>
-      <c r="AD4" s="15"/>
+      <c r="AD4" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE4" s="13">
         <v>5</v>
       </c>
@@ -1981,7 +2007,7 @@
       <c r="A5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -1996,7 +2022,7 @@
       <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -2047,10 +2073,10 @@
       <c r="W5" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X5" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="Y5" s="8" t="s">
+      <c r="X5" s="46">
+        <v>20</v>
+      </c>
+      <c r="Y5" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z5" s="8">
@@ -2094,7 +2120,7 @@
       <c r="A6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="40" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -2109,7 +2135,7 @@
       <c r="F6" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H6" s="13" t="s">
@@ -2154,14 +2180,16 @@
       <c r="U6" s="13">
         <v>4</v>
       </c>
-      <c r="V6" s="20" t="s">
+      <c r="V6" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="W6" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="13" t="s">
+      <c r="W6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="37" t="s">
         <v>18</v>
       </c>
       <c r="Z6" s="13">
@@ -2170,7 +2198,9 @@
       <c r="AA6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AB6" s="15"/>
+      <c r="AB6" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AC6" s="13">
         <v>72</v>
       </c>
@@ -2183,15 +2213,15 @@
       <c r="AF6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG6" s="21"/>
+      <c r="AG6" s="20"/>
       <c r="AH6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="AI6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ6" s="21"/>
-      <c r="AK6" s="22" t="s">
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="21" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2199,7 +2229,7 @@
       <c r="A7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2265,10 +2295,10 @@
       <c r="W7" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X7" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="Y7" s="8" t="s">
+      <c r="X7" s="46">
+        <v>20</v>
+      </c>
+      <c r="Y7" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z7" s="8">
@@ -2292,15 +2322,15 @@
       <c r="AF7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG7" s="23"/>
+      <c r="AG7" s="22"/>
       <c r="AH7" s="11" t="s">
         <v>21</v>
       </c>
       <c r="AI7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ7" s="23"/>
-      <c r="AK7" s="24" t="s">
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="23" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2308,7 +2338,7 @@
       <c r="A8" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -2323,19 +2353,21 @@
       <c r="F8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="37">
         <v>8</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="15">
+        <v>1</v>
+      </c>
       <c r="L8" s="13" t="s">
         <v>139</v>
       </c>
@@ -2372,10 +2404,10 @@
       <c r="W8" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X8" s="25">
-        <v>0.3</v>
-      </c>
-      <c r="Y8" s="13" t="s">
+      <c r="X8" s="46">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z8" s="13">
@@ -2390,22 +2422,24 @@
       <c r="AC8" s="13">
         <v>8</v>
       </c>
-      <c r="AD8" s="15"/>
+      <c r="AD8" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE8" s="13">
         <v>8</v>
       </c>
       <c r="AF8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG8" s="26"/>
+      <c r="AG8" s="24"/>
       <c r="AH8" s="17" t="s">
         <v>157</v>
       </c>
       <c r="AI8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ8" s="26"/>
-      <c r="AK8" s="27" t="s">
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="25" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2413,7 +2447,7 @@
       <c r="A9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="40" t="s">
         <v>234</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2479,8 +2513,10 @@
       <c r="W9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8" t="s">
+      <c r="X9" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z9" s="8">
@@ -2489,7 +2525,9 @@
       <c r="AA9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AB9" s="10"/>
+      <c r="AB9" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AC9" s="8">
         <v>84</v>
       </c>
@@ -2522,7 +2560,7 @@
       <c r="A10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2537,19 +2575,21 @@
       <c r="F10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="44">
+      <c r="I10" s="37">
         <v>119</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="15"/>
+      <c r="K10" s="15">
+        <v>1</v>
+      </c>
       <c r="L10" s="13" t="s">
         <v>4</v>
       </c>
@@ -2586,8 +2626,10 @@
       <c r="W10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="13" t="s">
+      <c r="X10" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="37" t="s">
         <v>18</v>
       </c>
       <c r="Z10" s="13">
@@ -2602,14 +2644,16 @@
       <c r="AC10" s="13">
         <v>119</v>
       </c>
-      <c r="AD10" s="15"/>
+      <c r="AD10" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE10" s="13">
         <v>9</v>
       </c>
       <c r="AF10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG10" s="21" t="s">
+      <c r="AG10" s="20" t="s">
         <v>121</v>
       </c>
       <c r="AH10" s="17" t="s">
@@ -2618,7 +2662,7 @@
       <c r="AI10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ10" s="21"/>
+      <c r="AJ10" s="20"/>
       <c r="AK10" s="18" t="s">
         <v>127</v>
       </c>
@@ -2627,7 +2671,7 @@
       <c r="A11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -2642,7 +2686,7 @@
       <c r="F11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -2693,10 +2737,10 @@
       <c r="W11" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X11" s="19">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Y11" s="8" t="s">
+      <c r="X11" s="46">
+        <v>28.000000000000004</v>
+      </c>
+      <c r="Y11" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z11" s="8">
@@ -2740,7 +2784,7 @@
       <c r="A12" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="40" t="s">
         <v>231</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -2752,22 +2796,24 @@
       <c r="E12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="37">
         <v>6</v>
       </c>
       <c r="J12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="15"/>
+      <c r="K12" s="15">
+        <v>1</v>
+      </c>
       <c r="L12" s="13" t="s">
         <v>139</v>
       </c>
@@ -2804,8 +2850,10 @@
       <c r="W12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="13" t="s">
+      <c r="X12" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="37" t="s">
         <v>18</v>
       </c>
       <c r="Z12" s="13">
@@ -2820,7 +2868,9 @@
       <c r="AC12" s="13">
         <v>6</v>
       </c>
-      <c r="AD12" s="15"/>
+      <c r="AD12" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE12" s="13">
         <v>6</v>
       </c>
@@ -2847,7 +2897,7 @@
       <c r="A13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -2862,7 +2912,7 @@
       <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H13" s="8" t="s">
@@ -2913,10 +2963,10 @@
       <c r="W13" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X13" s="28">
-        <v>1E-3</v>
-      </c>
-      <c r="Y13" s="8" t="s">
+      <c r="X13" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="Y13" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z13" s="8">
@@ -2960,7 +3010,7 @@
       <c r="A14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="40" t="s">
         <v>234</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2975,13 +3025,13 @@
       <c r="F14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="44">
+      <c r="I14" s="37">
         <v>120</v>
       </c>
       <c r="J14" s="13" t="s">
@@ -3026,8 +3076,10 @@
       <c r="W14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="13" t="s">
+      <c r="X14" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="37" t="s">
         <v>18</v>
       </c>
       <c r="Z14" s="13">
@@ -3042,14 +3094,16 @@
       <c r="AC14" s="13">
         <v>10</v>
       </c>
-      <c r="AD14" s="15"/>
+      <c r="AD14" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE14" s="13">
         <v>10</v>
       </c>
       <c r="AF14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG14" s="21" t="s">
+      <c r="AG14" s="20" t="s">
         <v>121</v>
       </c>
       <c r="AH14" s="17" t="s">
@@ -3058,7 +3112,7 @@
       <c r="AI14" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ14" s="21"/>
+      <c r="AJ14" s="20"/>
       <c r="AK14" s="18" t="s">
         <v>162</v>
       </c>
@@ -3067,7 +3121,7 @@
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="40" t="s">
         <v>231</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -3082,7 +3136,7 @@
       <c r="F15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H15" s="8" t="s">
@@ -3094,7 +3148,9 @@
       <c r="J15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10">
+        <v>1</v>
+      </c>
       <c r="L15" s="8" t="s">
         <v>139</v>
       </c>
@@ -3131,8 +3187,10 @@
       <c r="W15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="8" t="s">
+      <c r="X15" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z15" s="8">
@@ -3147,14 +3205,16 @@
       <c r="AC15" s="8">
         <v>7</v>
       </c>
-      <c r="AD15" s="8"/>
+      <c r="AD15" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="AE15" s="8">
         <v>7</v>
       </c>
       <c r="AF15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG15" s="23" t="s">
+      <c r="AG15" s="22" t="s">
         <v>121</v>
       </c>
       <c r="AH15" s="11" t="s">
@@ -3163,7 +3223,7 @@
       <c r="AI15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ15" s="23"/>
+      <c r="AJ15" s="22"/>
       <c r="AK15" s="12" t="s">
         <v>34</v>
       </c>
@@ -3172,7 +3232,7 @@
       <c r="A16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -3187,7 +3247,7 @@
       <c r="F16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H16" s="13" t="s">
@@ -3238,10 +3298,10 @@
       <c r="W16" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X16" s="30">
-        <v>0.2</v>
-      </c>
-      <c r="Y16" s="13" t="s">
+      <c r="X16" s="46">
+        <v>20</v>
+      </c>
+      <c r="Y16" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z16" s="13">
@@ -3265,7 +3325,7 @@
       <c r="AF16" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG16" s="31" t="s">
+      <c r="AG16" s="27" t="s">
         <v>227</v>
       </c>
       <c r="AH16" s="17" t="s">
@@ -3274,7 +3334,7 @@
       <c r="AI16" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AJ16" s="31" t="s">
+      <c r="AJ16" s="27" t="s">
         <v>35</v>
       </c>
       <c r="AK16" s="18" t="s">
@@ -3285,7 +3345,7 @@
       <c r="A17" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -3300,7 +3360,7 @@
       <c r="F17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H17" s="8" t="s">
@@ -3342,17 +3402,19 @@
       <c r="T17" s="8">
         <v>42</v>
       </c>
-      <c r="U17" s="10"/>
+      <c r="U17" s="10">
+        <v>0</v>
+      </c>
       <c r="V17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="W17" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X17" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="Y17" s="8" t="s">
+      <c r="X17" s="46">
+        <v>30</v>
+      </c>
+      <c r="Y17" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z17" s="8">
@@ -3367,7 +3429,9 @@
       <c r="AC17" s="8">
         <v>31</v>
       </c>
-      <c r="AD17" s="10"/>
+      <c r="AD17" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AE17" s="8">
         <v>31</v>
       </c>
@@ -3386,7 +3450,7 @@
       <c r="AJ17" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="AK17" s="32" t="s">
+      <c r="AK17" s="28" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3394,7 +3458,7 @@
       <c r="A18" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C18" s="13" t="s">
@@ -3406,16 +3470,16 @@
       <c r="E18" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="37">
         <v>36</v>
       </c>
       <c r="J18" s="13" t="s">
@@ -3460,8 +3524,10 @@
       <c r="W18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="13" t="s">
+      <c r="X18" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z18" s="13">
@@ -3476,12 +3542,16 @@
       <c r="AC18" s="13">
         <v>36</v>
       </c>
-      <c r="AD18" s="16"/>
-      <c r="AE18" s="33"/>
+      <c r="AD18" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE18" s="29">
+        <v>22</v>
+      </c>
       <c r="AF18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG18" s="21" t="s">
+      <c r="AG18" s="20" t="s">
         <v>121</v>
       </c>
       <c r="AH18" s="17" t="s">
@@ -3493,7 +3563,7 @@
       <c r="AJ18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="AK18" s="26" t="s">
+      <c r="AK18" s="24" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3501,7 +3571,7 @@
       <c r="A19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="40" t="s">
         <v>231</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -3516,7 +3586,7 @@
       <c r="F19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H19" s="8" t="s">
@@ -3528,7 +3598,9 @@
       <c r="J19" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="10">
+        <v>1</v>
+      </c>
       <c r="L19" s="8" t="s">
         <v>139</v>
       </c>
@@ -3565,8 +3637,10 @@
       <c r="W19" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="8" t="s">
+      <c r="X19" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z19" s="8">
@@ -3581,7 +3655,9 @@
       <c r="AC19" s="8">
         <v>2</v>
       </c>
-      <c r="AD19" s="29"/>
+      <c r="AD19" s="47" t="s">
+        <v>254</v>
+      </c>
       <c r="AE19" s="8">
         <v>33</v>
       </c>
@@ -3608,7 +3684,7 @@
       <c r="A20" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C20" s="13" t="s">
@@ -3635,7 +3711,9 @@
       <c r="J20" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="16">
+        <v>1</v>
+      </c>
       <c r="L20" s="13" t="s">
         <v>139</v>
       </c>
@@ -3672,10 +3750,10 @@
       <c r="W20" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X20" s="30">
-        <v>0.19</v>
-      </c>
-      <c r="Y20" s="13" t="s">
+      <c r="X20" s="46">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z20" s="13">
@@ -3719,7 +3797,7 @@
       <c r="A21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3734,7 +3812,7 @@
       <c r="F21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H21" s="8" t="s">
@@ -3785,10 +3863,10 @@
       <c r="W21" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X21" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="Y21" s="8" t="s">
+      <c r="X21" s="46">
+        <v>30</v>
+      </c>
+      <c r="Y21" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z21" s="8">
@@ -3803,7 +3881,9 @@
       <c r="AC21" s="8">
         <v>8</v>
       </c>
-      <c r="AD21" s="8"/>
+      <c r="AD21" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="AE21" s="8">
         <v>11</v>
       </c>
@@ -3819,7 +3899,7 @@
       <c r="AI21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ21" s="32"/>
+      <c r="AJ21" s="28"/>
       <c r="AK21" s="12" t="s">
         <v>41</v>
       </c>
@@ -3828,7 +3908,7 @@
       <c r="A22" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="40" t="s">
         <v>236</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -3843,7 +3923,7 @@
       <c r="F22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="38" t="s">
         <v>130</v>
       </c>
       <c r="H22" s="13" t="s">
@@ -3855,7 +3935,9 @@
       <c r="J22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="K22" s="15">
+        <v>1</v>
+      </c>
       <c r="L22" s="13" t="s">
         <v>139</v>
       </c>
@@ -3892,10 +3974,10 @@
       <c r="W22" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X22" s="34">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="Y22" s="13" t="s">
+      <c r="X22" s="46">
+        <v>3.75</v>
+      </c>
+      <c r="Y22" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z22" s="13">
@@ -3919,7 +4001,7 @@
       <c r="AF22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG22" s="21" t="s">
+      <c r="AG22" s="20" t="s">
         <v>121</v>
       </c>
       <c r="AH22" s="17" t="s">
@@ -3928,7 +4010,7 @@
       <c r="AI22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ22" s="26"/>
+      <c r="AJ22" s="24"/>
       <c r="AK22" s="18" t="s">
         <v>42</v>
       </c>
@@ -3937,7 +4019,7 @@
       <c r="A23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -3964,7 +4046,9 @@
       <c r="J23" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="29"/>
+      <c r="K23" s="26">
+        <v>1</v>
+      </c>
       <c r="L23" s="8" t="s">
         <v>139</v>
       </c>
@@ -3992,17 +4076,19 @@
       <c r="T23" s="8">
         <v>48</v>
       </c>
-      <c r="U23" s="10"/>
+      <c r="U23" s="10">
+        <v>0</v>
+      </c>
       <c r="V23" s="8" t="s">
         <v>17</v>
       </c>
       <c r="W23" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X23" s="19">
-        <v>0.24</v>
-      </c>
-      <c r="Y23" s="8" t="s">
+      <c r="X23" s="46">
+        <v>24</v>
+      </c>
+      <c r="Y23" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z23" s="8">
@@ -4017,7 +4103,9 @@
       <c r="AC23" s="8">
         <v>17</v>
       </c>
-      <c r="AD23" s="10"/>
+      <c r="AD23" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AE23" s="8">
         <v>17</v>
       </c>
@@ -4036,7 +4124,7 @@
       <c r="AJ23" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="AK23" s="32" t="s">
+      <c r="AK23" s="28" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4044,7 +4132,7 @@
       <c r="A24" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -4056,13 +4144,13 @@
       <c r="E24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>63</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="19" t="s">
         <v>188</v>
       </c>
       <c r="I24" s="13">
@@ -4072,7 +4160,7 @@
         <v>3</v>
       </c>
       <c r="K24" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="13" t="s">
         <v>12</v>
@@ -4110,8 +4198,10 @@
       <c r="W24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="13" t="s">
+      <c r="X24" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z24" s="13">
@@ -4120,7 +4210,9 @@
       <c r="AA24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AB24" s="15"/>
+      <c r="AB24" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AC24" s="13">
         <v>24</v>
       </c>
@@ -4142,8 +4234,8 @@
       <c r="AI24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ24" s="21"/>
-      <c r="AK24" s="35" t="s">
+      <c r="AJ24" s="20"/>
+      <c r="AK24" s="30" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4151,7 +4243,7 @@
       <c r="A25" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4166,10 +4258,10 @@
       <c r="F25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="41" t="s">
         <v>116</v>
       </c>
       <c r="I25" s="8">
@@ -4178,7 +4270,9 @@
       <c r="J25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="10"/>
+      <c r="K25" s="10">
+        <v>1</v>
+      </c>
       <c r="L25" s="8" t="s">
         <v>149</v>
       </c>
@@ -4215,8 +4309,10 @@
       <c r="W25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X25" s="29"/>
-      <c r="Y25" s="8" t="s">
+      <c r="X25" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z25" s="8">
@@ -4231,7 +4327,9 @@
       <c r="AC25" s="8">
         <v>7</v>
       </c>
-      <c r="AD25" s="10"/>
+      <c r="AD25" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AE25" s="8">
         <v>7</v>
       </c>
@@ -4250,7 +4348,7 @@
       <c r="AJ25" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AK25" s="32" t="s">
+      <c r="AK25" s="28" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4258,7 +4356,7 @@
       <c r="A26" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C26" s="13" t="s">
@@ -4273,7 +4371,7 @@
       <c r="F26" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="38" t="s">
         <v>48</v>
       </c>
       <c r="H26" s="13" t="s">
@@ -4285,7 +4383,9 @@
       <c r="J26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K26" s="16"/>
+      <c r="K26" s="16">
+        <v>1</v>
+      </c>
       <c r="L26" s="13" t="s">
         <v>50</v>
       </c>
@@ -4313,17 +4413,19 @@
       <c r="T26" s="13">
         <v>47.5</v>
       </c>
-      <c r="U26" s="15"/>
+      <c r="U26" s="15">
+        <v>0</v>
+      </c>
       <c r="V26" s="13" t="s">
         <v>14</v>
       </c>
       <c r="W26" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X26" s="30">
-        <v>0.05</v>
-      </c>
-      <c r="Y26" s="13" t="s">
+      <c r="X26" s="46">
+        <v>5</v>
+      </c>
+      <c r="Y26" s="37" t="s">
         <v>18</v>
       </c>
       <c r="Z26" s="13">
@@ -4347,7 +4449,7 @@
       <c r="AF26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG26" s="21" t="s">
+      <c r="AG26" s="20" t="s">
         <v>121</v>
       </c>
       <c r="AH26" s="17" t="s">
@@ -4356,8 +4458,8 @@
       <c r="AI26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ26" s="21"/>
-      <c r="AK26" s="35" t="s">
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="30" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4365,7 +4467,7 @@
       <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -4392,7 +4494,9 @@
       <c r="J27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="29"/>
+      <c r="K27" s="26">
+        <v>1</v>
+      </c>
       <c r="L27" s="8" t="s">
         <v>139</v>
       </c>
@@ -4429,8 +4533,10 @@
       <c r="W27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="8" t="s">
+      <c r="X27" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z27" s="8">
@@ -4445,14 +4551,16 @@
       <c r="AC27" s="8">
         <v>5</v>
       </c>
-      <c r="AD27" s="10"/>
+      <c r="AD27" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AE27" s="8">
         <v>5</v>
       </c>
       <c r="AF27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG27" s="23" t="s">
+      <c r="AG27" s="22" t="s">
         <v>121</v>
       </c>
       <c r="AH27" s="11" t="s">
@@ -4461,8 +4569,8 @@
       <c r="AI27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ27" s="23"/>
-      <c r="AK27" s="36" t="s">
+      <c r="AJ27" s="22"/>
+      <c r="AK27" s="31" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4470,7 +4578,7 @@
       <c r="A28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -4482,13 +4590,13 @@
       <c r="E28" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>63</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="19" t="s">
         <v>189</v>
       </c>
       <c r="I28" s="13">
@@ -4497,7 +4605,9 @@
       <c r="J28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="16"/>
+      <c r="K28" s="16">
+        <v>1</v>
+      </c>
       <c r="L28" s="13" t="s">
         <v>149</v>
       </c>
@@ -4534,8 +4644,10 @@
       <c r="W28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="13" t="s">
+      <c r="X28" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z28" s="13">
@@ -4550,14 +4662,16 @@
       <c r="AC28" s="13">
         <v>8</v>
       </c>
-      <c r="AD28" s="14"/>
+      <c r="AD28" s="14" t="s">
+        <v>254</v>
+      </c>
       <c r="AE28" s="13">
         <v>8</v>
       </c>
       <c r="AF28" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG28" s="31" t="s">
+      <c r="AG28" s="27" t="s">
         <v>169</v>
       </c>
       <c r="AH28" s="17" t="s">
@@ -4566,10 +4680,10 @@
       <c r="AI28" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AJ28" s="31" t="s">
+      <c r="AJ28" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="AK28" s="35" t="s">
+      <c r="AK28" s="30" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4577,7 +4691,7 @@
       <c r="A29" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -4604,7 +4718,9 @@
       <c r="J29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="29"/>
+      <c r="K29" s="26">
+        <v>1</v>
+      </c>
       <c r="L29" s="8" t="s">
         <v>139</v>
       </c>
@@ -4641,8 +4757,10 @@
       <c r="W29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X29" s="29"/>
-      <c r="Y29" s="8" t="s">
+      <c r="X29" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z29" s="8">
@@ -4657,14 +4775,16 @@
       <c r="AC29" s="8">
         <v>18</v>
       </c>
-      <c r="AD29" s="8"/>
+      <c r="AD29" s="8" t="s">
+        <v>254</v>
+      </c>
       <c r="AE29" s="8">
         <v>18</v>
       </c>
       <c r="AF29" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG29" s="32" t="s">
+      <c r="AG29" s="28" t="s">
         <v>121</v>
       </c>
       <c r="AH29" s="11" t="s">
@@ -4676,7 +4796,7 @@
       <c r="AJ29" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AK29" s="32" t="s">
+      <c r="AK29" s="28" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4684,7 +4804,7 @@
       <c r="A30" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C30" s="13" t="s">
@@ -4750,8 +4870,10 @@
       <c r="W30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="13" t="s">
+      <c r="X30" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z30" s="13">
@@ -4775,7 +4897,7 @@
       <c r="AF30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AG30" s="26" t="s">
+      <c r="AG30" s="24" t="s">
         <v>121</v>
       </c>
       <c r="AH30" s="17" t="s">
@@ -4784,8 +4906,8 @@
       <c r="AI30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ30" s="21"/>
-      <c r="AK30" s="27" t="s">
+      <c r="AJ30" s="20"/>
+      <c r="AK30" s="25" t="s">
         <v>121</v>
       </c>
     </row>
@@ -4793,7 +4915,7 @@
       <c r="A31" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -4820,7 +4942,9 @@
       <c r="J31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K31" s="10"/>
+      <c r="K31" s="10">
+        <v>1</v>
+      </c>
       <c r="L31" s="8" t="s">
         <v>139</v>
       </c>
@@ -4857,8 +4981,10 @@
       <c r="W31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X31" s="29"/>
-      <c r="Y31" s="8" t="s">
+      <c r="X31" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z31" s="8">
@@ -4882,7 +5008,7 @@
       <c r="AF31" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG31" s="23" t="s">
+      <c r="AG31" s="22" t="s">
         <v>121</v>
       </c>
       <c r="AH31" s="11" t="s">
@@ -4902,7 +5028,7 @@
       <c r="A32" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4914,13 +5040,13 @@
       <c r="E32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="19" t="s">
         <v>116</v>
       </c>
       <c r="I32" s="13">
@@ -4929,7 +5055,9 @@
       <c r="J32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K32" s="16"/>
+      <c r="K32" s="16">
+        <v>1</v>
+      </c>
       <c r="L32" s="13" t="s">
         <v>149</v>
       </c>
@@ -4966,8 +5094,10 @@
       <c r="W32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="13" t="s">
+      <c r="X32" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z32" s="13">
@@ -4982,14 +5112,16 @@
       <c r="AC32" s="13">
         <v>6</v>
       </c>
-      <c r="AD32" s="15"/>
+      <c r="AD32" s="43" t="s">
+        <v>254</v>
+      </c>
       <c r="AE32" s="13">
         <v>6</v>
       </c>
       <c r="AF32" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG32" s="31" t="s">
+      <c r="AG32" s="27" t="s">
         <v>250</v>
       </c>
       <c r="AH32" s="17" t="s">
@@ -4998,7 +5130,7 @@
       <c r="AI32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ32" s="21"/>
+      <c r="AJ32" s="20"/>
       <c r="AK32" s="18" t="s">
         <v>54</v>
       </c>
@@ -5007,7 +5139,7 @@
       <c r="A33" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="40" t="s">
         <v>236</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -5073,8 +5205,10 @@
       <c r="W33" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X33" s="29"/>
-      <c r="Y33" s="8" t="s">
+      <c r="X33" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="41" t="s">
         <v>18</v>
       </c>
       <c r="Z33" s="8">
@@ -5083,18 +5217,22 @@
       <c r="AA33" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AB33" s="10"/>
+      <c r="AB33" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AC33" s="8">
         <v>166</v>
       </c>
-      <c r="AD33" s="29"/>
+      <c r="AD33" s="47" t="s">
+        <v>254</v>
+      </c>
       <c r="AE33" s="8">
         <v>48</v>
       </c>
       <c r="AF33" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG33" s="32" t="s">
+      <c r="AG33" s="28" t="s">
         <v>121</v>
       </c>
       <c r="AH33" s="11" t="s">
@@ -5114,7 +5252,7 @@
       <c r="A34" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -5129,10 +5267,10 @@
       <c r="F34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="47" t="s">
+      <c r="G34" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H34" s="44" t="s">
+      <c r="H34" s="37" t="s">
         <v>134</v>
       </c>
       <c r="I34" s="13">
@@ -5180,8 +5318,10 @@
       <c r="W34" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X34" s="16"/>
-      <c r="Y34" s="13" t="s">
+      <c r="X34" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z34" s="13">
@@ -5196,14 +5336,16 @@
       <c r="AC34" s="13">
         <v>12</v>
       </c>
-      <c r="AD34" s="14"/>
+      <c r="AD34" s="14" t="s">
+        <v>254</v>
+      </c>
       <c r="AE34" s="13">
         <v>24</v>
       </c>
       <c r="AF34" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG34" s="31" t="s">
+      <c r="AG34" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AH34" s="17" t="s">
@@ -5215,7 +5357,7 @@
       <c r="AJ34" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="AK34" s="21" t="s">
+      <c r="AK34" s="20" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5223,7 +5365,7 @@
       <c r="A35" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -5238,7 +5380,7 @@
       <c r="F35" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="45" t="s">
+      <c r="G35" s="38" t="s">
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
@@ -5289,10 +5431,10 @@
       <c r="W35" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="X35" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="Y35" s="8" t="s">
+      <c r="X35" s="46">
+        <v>20</v>
+      </c>
+      <c r="Y35" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z35" s="8">
@@ -5325,7 +5467,7 @@
       <c r="AI35" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ35" s="32"/>
+      <c r="AJ35" s="28"/>
       <c r="AK35" s="12" t="s">
         <v>143</v>
       </c>
@@ -5334,7 +5476,7 @@
       <c r="A36" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C36" s="13" t="s">
@@ -5400,8 +5542,10 @@
       <c r="W36" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="13" t="s">
+      <c r="X36" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z36" s="13">
@@ -5434,7 +5578,7 @@
       <c r="AI36" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AJ36" s="31" t="s">
+      <c r="AJ36" s="27" t="s">
         <v>59</v>
       </c>
       <c r="AK36" s="18" t="s">
@@ -5445,7 +5589,7 @@
       <c r="A37" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="40" t="s">
         <v>231</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -5511,8 +5655,10 @@
       <c r="W37" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8" t="s">
+      <c r="X37" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="41" t="s">
         <v>10</v>
       </c>
       <c r="Z37" s="8">
@@ -5536,7 +5682,7 @@
       <c r="AF37" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG37" s="32" t="s">
+      <c r="AG37" s="28" t="s">
         <v>121</v>
       </c>
       <c r="AH37" s="11" t="s">
@@ -5548,7 +5694,7 @@
       <c r="AJ37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AK37" s="32" t="s">
+      <c r="AK37" s="28" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5556,7 +5702,7 @@
       <c r="A38" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C38" s="13" t="s">
@@ -5574,16 +5720,18 @@
       <c r="G38" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I38" s="44">
+      <c r="I38" s="37">
         <v>30</v>
       </c>
       <c r="J38" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K38" s="13"/>
+      <c r="K38" s="13">
+        <v>1</v>
+      </c>
       <c r="L38" s="13" t="s">
         <v>12</v>
       </c>
@@ -5620,10 +5768,10 @@
       <c r="W38" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X38" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="Y38" s="13" t="s">
+      <c r="X38" s="46">
+        <v>10</v>
+      </c>
+      <c r="Y38" s="37" t="s">
         <v>10</v>
       </c>
       <c r="Z38" s="13">
@@ -5638,14 +5786,16 @@
       <c r="AC38" s="13">
         <v>30</v>
       </c>
-      <c r="AD38" s="13"/>
+      <c r="AD38" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="AE38" s="13">
         <v>30</v>
       </c>
       <c r="AF38" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG38" s="31" t="s">
+      <c r="AG38" s="27" t="s">
         <v>60</v>
       </c>
       <c r="AH38" s="17" t="s">
@@ -5657,7 +5807,7 @@
       <c r="AJ38" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="AK38" s="35" t="s">
+      <c r="AK38" s="30" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5665,7 +5815,7 @@
       <c r="A39" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -5680,10 +5830,10 @@
       <c r="F39" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="47" t="s">
+      <c r="G39" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="48" t="s">
+      <c r="H39" s="41" t="s">
         <v>61</v>
       </c>
       <c r="I39" s="8">
@@ -5692,7 +5842,9 @@
       <c r="J39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K39" s="10"/>
+      <c r="K39" s="10">
+        <v>1</v>
+      </c>
       <c r="L39" s="8" t="s">
         <v>144</v>
       </c>
@@ -5729,8 +5881,10 @@
       <c r="W39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X39" s="10"/>
-      <c r="Y39" s="8" t="s">
+      <c r="X39" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z39" s="8">
@@ -5739,7 +5893,9 @@
       <c r="AA39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AB39" s="10"/>
+      <c r="AB39" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="AC39" s="8">
         <v>96</v>
       </c>
@@ -5752,7 +5908,7 @@
       <c r="AF39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG39" s="32" t="s">
+      <c r="AG39" s="28" t="s">
         <v>121</v>
       </c>
       <c r="AH39" s="11" t="s">
@@ -5761,8 +5917,8 @@
       <c r="AI39" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AJ39" s="32"/>
-      <c r="AK39" s="36" t="s">
+      <c r="AJ39" s="28"/>
+      <c r="AK39" s="31" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5770,7 +5926,7 @@
       <c r="A40" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="40" t="s">
         <v>233</v>
       </c>
       <c r="C40" s="13" t="s">
@@ -5785,7 +5941,7 @@
       <c r="F40" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="45" t="s">
+      <c r="G40" s="38" t="s">
         <v>48</v>
       </c>
       <c r="H40" s="13" t="s">
@@ -5836,10 +5992,10 @@
       <c r="W40" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="X40" s="30">
-        <v>0.3</v>
-      </c>
-      <c r="Y40" s="13" t="s">
+      <c r="X40" s="46">
+        <v>30</v>
+      </c>
+      <c r="Y40" s="37" t="s">
         <v>6</v>
       </c>
       <c r="Z40" s="13">
@@ -5848,7 +6004,9 @@
       <c r="AA40" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AB40" s="16"/>
+      <c r="AB40" s="44" t="s">
+        <v>254</v>
+      </c>
       <c r="AC40" s="13">
         <v>8</v>
       </c>
@@ -5861,7 +6019,7 @@
       <c r="AF40" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AG40" s="31" t="s">
+      <c r="AG40" s="27" t="s">
         <v>180</v>
       </c>
       <c r="AH40" s="17" t="s">
@@ -5870,10 +6028,10 @@
       <c r="AI40" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AJ40" s="31" t="s">
+      <c r="AJ40" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="AK40" s="35" t="s">
+      <c r="AK40" s="30" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5881,7 +6039,7 @@
       <c r="A41" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="40" t="s">
         <v>235</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -5908,7 +6066,9 @@
       <c r="J41" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K41" s="10"/>
+      <c r="K41" s="10">
+        <v>1</v>
+      </c>
       <c r="L41" s="8" t="s">
         <v>12</v>
       </c>
@@ -5936,15 +6096,19 @@
       <c r="T41" s="8">
         <v>40</v>
       </c>
-      <c r="U41" s="10"/>
+      <c r="U41" s="10">
+        <v>0</v>
+      </c>
       <c r="V41" s="8" t="s">
         <v>17</v>
       </c>
       <c r="W41" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X41" s="10"/>
-      <c r="Y41" s="8" t="s">
+      <c r="X41" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Z41" s="8">
@@ -5968,7 +6132,7 @@
       <c r="AF41" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AG41" s="32" t="s">
+      <c r="AG41" s="28" t="s">
         <v>121</v>
       </c>
       <c r="AH41" s="11" t="s">
@@ -5980,117 +6144,122 @@
       <c r="AJ41" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="AK41" s="32" t="s">
+      <c r="AK41" s="28" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="C42" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="37" t="s">
+      <c r="C42" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="E42" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="F42" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="H42" s="37" t="s">
+      <c r="H42" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="I42" s="37">
-        <v>4</v>
-      </c>
-      <c r="J42" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="K42" s="38"/>
-      <c r="L42" s="37" t="s">
+      <c r="I42" s="32">
+        <v>4</v>
+      </c>
+      <c r="J42" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" s="33">
+        <v>1</v>
+      </c>
+      <c r="L42" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="M42" s="37">
-        <v>3</v>
-      </c>
-      <c r="N42" s="37">
-        <v>3</v>
-      </c>
-      <c r="O42" s="37">
-        <v>3</v>
-      </c>
-      <c r="P42" s="37">
-        <v>3</v>
-      </c>
-      <c r="Q42" s="37" t="s">
+      <c r="M42" s="32">
+        <v>3</v>
+      </c>
+      <c r="N42" s="32">
+        <v>3</v>
+      </c>
+      <c r="O42" s="32">
+        <v>3</v>
+      </c>
+      <c r="P42" s="32">
+        <v>3</v>
+      </c>
+      <c r="Q42" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="R42" s="37">
-        <v>4</v>
-      </c>
-      <c r="S42" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="T42" s="37">
+      <c r="R42" s="32">
+        <v>4</v>
+      </c>
+      <c r="S42" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="T42" s="32">
         <v>25</v>
       </c>
-      <c r="U42" s="38">
+      <c r="U42" s="33">
         <v>1.5</v>
       </c>
-      <c r="V42" s="37" t="s">
+      <c r="V42" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="W42" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="X42" s="39"/>
-      <c r="Y42" s="37" t="s">
+      <c r="W42" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="X42" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="Z42" s="37">
-        <v>4</v>
-      </c>
-      <c r="AA42" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB42" s="37">
-        <v>3</v>
-      </c>
-      <c r="AC42" s="37">
-        <v>4</v>
-      </c>
-      <c r="AD42" s="40"/>
-      <c r="AE42" s="41">
-        <v>4</v>
-      </c>
-      <c r="AF42" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG42" s="42" t="s">
+      <c r="Z42" s="32">
+        <v>4</v>
+      </c>
+      <c r="AA42" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB42" s="32">
+        <v>3</v>
+      </c>
+      <c r="AC42" s="32">
+        <v>4</v>
+      </c>
+      <c r="AD42" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE42" s="34">
+        <v>4</v>
+      </c>
+      <c r="AF42" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG42" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="AH42" s="43" t="s">
+      <c r="AH42" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="AI42" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ42" s="21"/>
-      <c r="AK42" s="27" t="s">
+      <c r="AI42" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ42" s="20"/>
+      <c r="AK42" s="25" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en survey_ready.xlsx y survey_analysis.ipynb
</commit_message>
<xml_diff>
--- a/data/raw/survey_ready.xlsx
+++ b/data/raw/survey_ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610DC131-37AC-4EF7-A49F-8D93841E1F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957F8AF3-7635-4DEE-A052-EB1B47F035A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,12 +422,6 @@
     <t>Tecnico</t>
   </si>
   <si>
-    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Factores personales (salud, estres, etc.)</t>
-  </si>
-  <si>
-    <t>Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Factores personales (salud, estres, etc.)</t>
-  </si>
-  <si>
     <t>Compras, almacen, cxp</t>
   </si>
   <si>
@@ -467,9 +461,6 @@
     <t>Considero que seria importante establecer limites en cuanto a las opiniones y cambios sobre areas que no estan a su cargo. ademas, seria beneficioso contar con un gerente general que sea el encargado de tomar las decisiones finales en estos temas. esto contribuiria a que cada area tenga la autonomia y el respeto necesarios para funcionar de manera mas eficiente, reduciendo posibles conflictos y aumentando la satisfaccion laboral.</t>
   </si>
   <si>
-    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional, Ambiente laboral</t>
-  </si>
-  <si>
     <t>El ambiente laboral, los constantes cambios de procesos, la carga de trabajo y la falta de reconocimiento son factores clave que afectan mi experiencia en la empresa. estos aspectos dificultan la motivacion y el compromiso, ya que no se percibe el apoyo necesario ni un ambiente que valore el esfuerzo realizado.</t>
   </si>
   <si>
@@ -482,31 +473,16 @@
     <t xml:space="preserve">Delimitar alcances dentro de las funsiones de la direccion, imparcialidad e vitar el conflicto de interes en la toma de deciciones </t>
   </si>
   <si>
-    <t>Oferta laboral en otras empresas, Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional, Ambiente laboral, Factores personales (salud, estres, etc.)</t>
-  </si>
-  <si>
     <t>Conflicto de intereses entre la direccion, falta de transparencia y etica laboral, la directriz cambia sin previo aviso y la comunicacion no es eficiente</t>
   </si>
   <si>
-    <t>Oferta laboral en otras empresas, Distancia entre casa y trabajo, Falta de transporte adecuado, Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Ambiente laboral, Factores personales (salud, estres, etc.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Metrologo </t>
   </si>
   <si>
-    <t>Oferta laboral en otras empresas, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional</t>
-  </si>
-  <si>
     <t>Contratacion de personal competente</t>
   </si>
   <si>
-    <t>Responsabilidades familiares, Condiciones economicas generales (inflacion, costo de vida, etc.)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Por crecimiento profesional y economico </t>
-  </si>
-  <si>
-    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales (inflacion, costo de vida, etc.)</t>
   </si>
   <si>
     <t>Que la empresa ofresca incentivos economicos a sus empleados por ejemplo: comedor industrial, transporte para los empleados, premios de productividad, caja de ahorro, vales de despensas, aumento de salario , uniformes, capacitaciones externas, seguro de gasta medicos mayores, etc.</t>
@@ -523,9 +499,6 @@
   <si>
     <t xml:space="preserve">Considero que el ambiente laboral dentro de la empresa es bueno pero creo que implementar actividades o cierto tipo de dinamicas no estaria mal para que logremos entender que el trabajo en equipo entre todas las areas es fundamental para un crecimiento, saber que si a la empresa le va bien, a las areas nos va bien 
 tambien considero que la adquisicion de nuevos equipos ayudaria a atraer a mas clientes </t>
-  </si>
-  <si>
-    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional, Ambiente laboral, Factores personales (salud, estres, etc.), Otro</t>
   </si>
   <si>
     <t>Se generan comentarios de humillacion y desmotivacion, asi como menosprecio y desvalorizan el trabajo realizado y concluido satisfactoriamente, para con ello justificar el incumpliendo de las responsabilidades con los colaboradores. se da prioridad a gastos innecesarios o poco relevantes en en vez de enfocarse a destinar los recursos a las necesidades mas importantes y urgentes de la empresa y de los colaboradores</t>
@@ -546,19 +519,10 @@
     <t xml:space="preserve">Reconocimiento al trabajo efectuado por el colaborador e incentivarlo y motivarlo monetariamente o alguna otra prestacion de acuerdo a las de ley. </t>
   </si>
   <si>
-    <t>Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Ambiente laboral</t>
-  </si>
-  <si>
-    <t>Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Ambiente laboral</t>
-  </si>
-  <si>
     <t xml:space="preserve">Considero que hace falta mas atencion hacia el personal y no precisamente incentivos economicos si no que se debe mejorar la relacion empleado-empresa, debe ser mutuo. y seguir mejorando la imagen. </t>
   </si>
   <si>
     <t xml:space="preserve">Incentivos de pertenencia hacia la empresa, economicos, reconocimientos por logros, mejoras, agradecimientos etc. </t>
-  </si>
-  <si>
-    <t>Salario poco competitivo en el mercado, Condiciones economicas generales (inflacion, costo de vida, etc.), Otro</t>
   </si>
   <si>
     <t xml:space="preserve">Facturacion </t>
@@ -571,19 +535,10 @@
 mas alla del salario, que en su momento me hicieron dudar de continuar mi estancia aqui; poniendolo en la balanza; ha sido basto el apoyo que he recibido dentro de la empresa en cuestiones personales, cuando por emergencias con mi hija, me ha tocado abrir el dialogo para encontrar otros caminos para no descuidar ambos aspectos; y profesionales al darme la oportunidad de ir creciendo dentro de la empresa.</t>
   </si>
   <si>
-    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales (inflacion, costo de vida, etc.), Ambiente laboral</t>
-  </si>
-  <si>
     <t>Se ha frenado, por parte de personal perteneciente a la direccion, cualquier intento de implementar la estrategia de datos en la empresa, incluso con faltas de respeto hacia mi persona, lo cual impide cualquier intento de crecimiento y aumenta la frustracion.</t>
   </si>
   <si>
-    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Responsabilidades familiares, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional, Ambiente laboral</t>
-  </si>
-  <si>
     <t>Si, diria que he observado como la falta de consecuencias equitativas ante errores graves genera un sentimiento de injusticia que se puede palpar claramente. es como si algunos cargaran con todo el peso, mientras que otros siguen adelante sin asumir responsabilidad. esto, inevitablemente, lastima la confianza entre nosotros, los colaboradores, y dificulta la colaboracion. se siente un ambiente de desanimo, donde la motivacion disminuye y el trabajo en equipo se resiente. creo que todos merecemos un trato justo, y que aprender de los errores, juntos, nos haria mas fuertes como equipo.</t>
-  </si>
-  <si>
-    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales (inflacion, costo de vida, etc.), Falta de oportunidades de crecimiento profesional</t>
   </si>
   <si>
     <t>Dentro del giro metrologico es una buena empresa y respetada por la eficiencia en sus servicios, desafortunadamente las expectativas cambiaron al ver ciertas acciones que se llevan a cabo y no son de algun modo profesionales, eticas al momento de dirigirse con el personal. 
@@ -807,6 +762,51 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional, Ambiente laboral</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional</t>
+  </si>
+  <si>
+    <t>Responsabilidades familiares, Condiciones economicas generales</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales</t>
+  </si>
+  <si>
+    <t>Salario poco competitivo en el mercado, Condiciones economicas generales, Ambiente laboral</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Condiciones economicas generales, Ambiente laboral</t>
+  </si>
+  <si>
+    <t>Salario poco competitivo en el mercado, Condiciones economicas generales, Otro</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales, Ambiente laboral</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Responsabilidades familiares, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional, Ambiente laboral</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional, Ambiente laboral, Factores personales</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Distancia entre casa y trabajo, Falta de transporte adecuado, Salario poco competitivo en el mercado, Condiciones economicas generales, Ambiente laboral, Factores personales</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Responsabilidades familiares, Factores personales</t>
+  </si>
+  <si>
+    <t>Oferta laboral en otras empresas, Salario poco competitivo en el mercado, Condiciones economicas generales, Falta de oportunidades de crecimiento profesional, Ambiente laboral, Factores personales, Otro</t>
+  </si>
+  <si>
+    <t>Distancia entre casa y trabajo, Salario poco competitivo en el mercado, Factores personales</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1247,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1504,9 +1504,9 @@
   </sheetPr>
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1553,115 +1553,115 @@
   <sheetData>
     <row r="1" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AK1" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="158.4" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -1747,34 +1747,34 @@
         <v>3</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC2" s="5">
         <v>70</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE2" s="5">
         <v>48</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>147</v>
+        <v>240</v>
       </c>
       <c r="AK2" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="92.4" x14ac:dyDescent="0.25">
@@ -1782,7 +1782,7 @@
         <v>72</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>7</v>
@@ -1800,19 +1800,19 @@
         <v>48</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I3" s="8">
         <v>109</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K3" s="8">
         <v>5</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M3" s="8">
         <v>3</v>
@@ -1860,7 +1860,7 @@
         <v>3</v>
       </c>
       <c r="AB3" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC3" s="8">
         <v>48</v>
@@ -1872,22 +1872,22 @@
         <v>84</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AH3" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ3" s="11" t="s">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:37" ht="92.4" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>7</v>
@@ -1946,7 +1946,7 @@
         <v>3</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T4" s="13">
         <v>50</v>
@@ -1970,7 +1970,7 @@
         <v>3</v>
       </c>
       <c r="AA4" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB4" s="14">
         <v>4</v>
@@ -1979,28 +1979,28 @@
         <v>29</v>
       </c>
       <c r="AD4" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE4" s="13">
         <v>5</v>
       </c>
       <c r="AF4" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG4" s="17" t="s">
         <v>15</v>
       </c>
       <c r="AH4" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AI4" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ4" s="17" t="s">
-        <v>154</v>
+        <v>251</v>
       </c>
       <c r="AK4" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>7</v>
@@ -2026,13 +2026,13 @@
         <v>130</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I5" s="8">
         <v>34</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K5" s="8">
         <v>2</v>
@@ -2053,7 +2053,7 @@
         <v>4</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R5" s="8">
         <v>4</v>
@@ -2071,7 +2071,7 @@
         <v>17</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X5" s="46">
         <v>20</v>
@@ -2083,7 +2083,7 @@
         <v>3</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB5" s="8">
         <v>4</v>
@@ -2098,22 +2098,22 @@
         <v>9</v>
       </c>
       <c r="AF5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="AH5" s="11" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ5" s="11" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>0</v>
@@ -2139,19 +2139,19 @@
         <v>130</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I6" s="13">
         <v>254</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K6" s="13">
         <v>3</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M6" s="13">
         <v>0</v>
@@ -2199,7 +2199,7 @@
         <v>3</v>
       </c>
       <c r="AB6" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC6" s="13">
         <v>72</v>
@@ -2230,7 +2230,7 @@
         <v>76</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>7</v>
@@ -2248,19 +2248,19 @@
         <v>20</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I7" s="8">
         <v>34</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K7" s="8">
         <v>2</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M7" s="8">
         <v>1</v>
@@ -2275,13 +2275,13 @@
         <v>5</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R7" s="8">
         <v>4</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T7" s="8">
         <v>41</v>
@@ -2293,7 +2293,7 @@
         <v>17</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X7" s="46">
         <v>20</v>
@@ -2305,7 +2305,7 @@
         <v>1.5</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB7" s="8">
         <v>5</v>
@@ -2339,7 +2339,7 @@
         <v>77</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>7</v>
@@ -2369,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M8" s="13">
         <v>2</v>
@@ -2384,13 +2384,13 @@
         <v>4</v>
       </c>
       <c r="Q8" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R8" s="13">
         <v>4</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T8" s="13">
         <v>48</v>
@@ -2402,7 +2402,7 @@
         <v>14</v>
       </c>
       <c r="W8" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X8" s="46">
         <v>30</v>
@@ -2414,7 +2414,7 @@
         <v>3</v>
       </c>
       <c r="AA8" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB8" s="13">
         <v>5</v>
@@ -2423,7 +2423,7 @@
         <v>8</v>
       </c>
       <c r="AD8" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE8" s="13">
         <v>8</v>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="AG8" s="24"/>
       <c r="AH8" s="17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="AI8" s="13" t="s">
         <v>3</v>
@@ -2448,7 +2448,7 @@
         <v>78</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>0</v>
@@ -2466,19 +2466,19 @@
         <v>22</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I9" s="8">
         <v>252</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K9" s="8">
         <v>2</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M9" s="8">
         <v>3</v>
@@ -2493,7 +2493,7 @@
         <v>5</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R9" s="8">
         <v>4</v>
@@ -2526,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="AB9" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC9" s="8">
         <v>84</v>
@@ -2544,16 +2544,16 @@
         <v>119</v>
       </c>
       <c r="AH9" s="11" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ9" s="11" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
@@ -2561,7 +2561,7 @@
         <v>79</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>7</v>
@@ -2606,13 +2606,13 @@
         <v>5</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R10" s="13">
         <v>4</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T10" s="13">
         <v>47</v>
@@ -2636,7 +2636,7 @@
         <v>2</v>
       </c>
       <c r="AA10" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB10" s="14">
         <v>5</v>
@@ -2645,7 +2645,7 @@
         <v>119</v>
       </c>
       <c r="AD10" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE10" s="13">
         <v>9</v>
@@ -2672,7 +2672,7 @@
         <v>80</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>7</v>
@@ -2696,13 +2696,13 @@
         <v>36</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K11" s="8">
         <v>2</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M11" s="8">
         <v>3</v>
@@ -2717,7 +2717,7 @@
         <v>5</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R11" s="8">
         <v>4</v>
@@ -2735,7 +2735,7 @@
         <v>14</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X11" s="46">
         <v>28.000000000000004</v>
@@ -2747,7 +2747,7 @@
         <v>5</v>
       </c>
       <c r="AA11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB11" s="8">
         <v>4</v>
@@ -2762,22 +2762,22 @@
         <v>36</v>
       </c>
       <c r="AF11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="AH11" s="11" t="s">
         <v>23</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ11" s="11" t="s">
-        <v>160</v>
+        <v>243</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
@@ -2785,7 +2785,7 @@
         <v>81</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>7</v>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M12" s="13">
         <v>1</v>
@@ -2860,7 +2860,7 @@
         <v>6</v>
       </c>
       <c r="AA12" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB12" s="13">
         <v>4</v>
@@ -2869,13 +2869,13 @@
         <v>6</v>
       </c>
       <c r="AD12" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE12" s="13">
         <v>6</v>
       </c>
       <c r="AF12" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG12" s="17" t="s">
         <v>25</v>
@@ -2884,13 +2884,13 @@
         <v>26</v>
       </c>
       <c r="AI12" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ12" s="17" t="s">
         <v>27</v>
       </c>
       <c r="AK12" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
@@ -2898,7 +2898,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>7</v>
@@ -2922,13 +2922,13 @@
         <v>106</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K13" s="8">
         <v>4</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M13" s="8">
         <v>7</v>
@@ -2943,13 +2943,13 @@
         <v>3</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R13" s="8">
         <v>4</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T13" s="8">
         <v>43</v>
@@ -2961,7 +2961,7 @@
         <v>14</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X13" s="46">
         <v>0.1</v>
@@ -2973,7 +2973,7 @@
         <v>2.5</v>
       </c>
       <c r="AA13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB13" s="8">
         <v>3</v>
@@ -2988,16 +2988,16 @@
         <v>72</v>
       </c>
       <c r="AF13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG13" s="11" t="s">
         <v>45</v>
       </c>
       <c r="AH13" s="11" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ13" s="11" t="s">
         <v>28</v>
@@ -3011,7 +3011,7 @@
         <v>83</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>7</v>
@@ -3035,7 +3035,7 @@
         <v>120</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K14" s="13">
         <v>2</v>
@@ -3056,13 +3056,13 @@
         <v>5</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R14" s="13">
         <v>4</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T14" s="13">
         <v>49</v>
@@ -3086,7 +3086,7 @@
         <v>5</v>
       </c>
       <c r="AA14" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB14" s="13">
         <v>5</v>
@@ -3095,7 +3095,7 @@
         <v>10</v>
       </c>
       <c r="AD14" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE14" s="13">
         <v>10</v>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="AJ14" s="20"/>
       <c r="AK14" s="18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>84</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>0</v>
@@ -3152,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M15" s="8">
         <v>2</v>
@@ -3167,13 +3167,13 @@
         <v>3</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R15" s="8">
         <v>5</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T15" s="8">
         <v>25</v>
@@ -3197,7 +3197,7 @@
         <v>1</v>
       </c>
       <c r="AA15" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB15" s="8">
         <v>4</v>
@@ -3206,7 +3206,7 @@
         <v>7</v>
       </c>
       <c r="AD15" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE15" s="8">
         <v>7</v>
@@ -3233,7 +3233,7 @@
         <v>85</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>0</v>
@@ -3257,13 +3257,13 @@
         <v>65</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K16" s="14">
         <v>3</v>
       </c>
       <c r="L16" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M16" s="13">
         <v>1</v>
@@ -3278,7 +3278,7 @@
         <v>4</v>
       </c>
       <c r="Q16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R16" s="13">
         <v>4</v>
@@ -3296,7 +3296,7 @@
         <v>5</v>
       </c>
       <c r="W16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X16" s="46">
         <v>20</v>
@@ -3308,7 +3308,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB16" s="13">
         <v>3</v>
@@ -3323,22 +3323,22 @@
         <v>63</v>
       </c>
       <c r="AF16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG16" s="27" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="AH16" s="17" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="AI16" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ16" s="27" t="s">
         <v>35</v>
       </c>
       <c r="AK16" s="18" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
@@ -3346,13 +3346,13 @@
         <v>86</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>131</v>
@@ -3370,13 +3370,13 @@
         <v>31</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K17" s="8">
         <v>2</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M17" s="8">
         <v>2</v>
@@ -3391,7 +3391,7 @@
         <v>4</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R17" s="8">
         <v>2</v>
@@ -3409,7 +3409,7 @@
         <v>14</v>
       </c>
       <c r="W17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X17" s="46">
         <v>30</v>
@@ -3421,7 +3421,7 @@
         <v>4.5</v>
       </c>
       <c r="AA17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB17" s="8">
         <v>4</v>
@@ -3430,13 +3430,13 @@
         <v>31</v>
       </c>
       <c r="AD17" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE17" s="8">
         <v>31</v>
       </c>
       <c r="AF17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG17" s="11" t="s">
         <v>37</v>
@@ -3445,10 +3445,10 @@
         <v>123</v>
       </c>
       <c r="AI17" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ17" s="11" t="s">
-        <v>132</v>
+        <v>252</v>
       </c>
       <c r="AK17" s="28" t="s">
         <v>121</v>
@@ -3459,7 +3459,7 @@
         <v>87</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>0</v>
@@ -3483,7 +3483,7 @@
         <v>36</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K18" s="13">
         <v>2</v>
@@ -3504,7 +3504,7 @@
         <v>4</v>
       </c>
       <c r="Q18" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R18" s="13">
         <v>4</v>
@@ -3534,7 +3534,7 @@
         <v>1.5</v>
       </c>
       <c r="AA18" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB18" s="13">
         <v>4</v>
@@ -3543,7 +3543,7 @@
         <v>36</v>
       </c>
       <c r="AD18" s="44" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE18" s="29">
         <v>22</v>
@@ -3558,7 +3558,7 @@
         <v>112</v>
       </c>
       <c r="AI18" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ18" s="17" t="s">
         <v>38</v>
@@ -3572,7 +3572,7 @@
         <v>88</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>0</v>
@@ -3602,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M19" s="8">
         <v>0</v>
@@ -3617,13 +3617,13 @@
         <v>4</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R19" s="8">
         <v>3</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T19" s="8">
         <v>45</v>
@@ -3635,7 +3635,7 @@
         <v>14</v>
       </c>
       <c r="W19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X19" s="46">
         <v>0</v>
@@ -3647,7 +3647,7 @@
         <v>2</v>
       </c>
       <c r="AA19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB19" s="8">
         <v>3</v>
@@ -3656,28 +3656,28 @@
         <v>2</v>
       </c>
       <c r="AD19" s="47" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE19" s="8">
         <v>33</v>
       </c>
       <c r="AF19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG19" s="11" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="AH19" s="11" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="AI19" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ19" s="11" t="s">
         <v>39</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:37" ht="145.19999999999999" x14ac:dyDescent="0.25">
@@ -3685,7 +3685,7 @@
         <v>89</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>0</v>
@@ -3703,7 +3703,7 @@
         <v>20</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I20" s="13">
         <v>27</v>
@@ -3715,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M20" s="13">
         <v>4</v>
@@ -3736,7 +3736,7 @@
         <v>2</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T20" s="13">
         <v>48</v>
@@ -3748,7 +3748,7 @@
         <v>17</v>
       </c>
       <c r="W20" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X20" s="46">
         <v>19</v>
@@ -3760,7 +3760,7 @@
         <v>1</v>
       </c>
       <c r="AA20" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB20" s="13">
         <v>3</v>
@@ -3775,22 +3775,22 @@
         <v>20</v>
       </c>
       <c r="AF20" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG20" s="17" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="AH20" s="17" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="AI20" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ20" s="17" t="s">
-        <v>166</v>
+        <v>253</v>
       </c>
       <c r="AK20" s="18" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
         <v>90</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>0</v>
@@ -3822,7 +3822,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K21" s="8">
         <v>2</v>
@@ -3843,13 +3843,13 @@
         <v>5</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R21" s="8">
         <v>4</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T21" s="8">
         <v>48</v>
@@ -3861,7 +3861,7 @@
         <v>14</v>
       </c>
       <c r="W21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X21" s="46">
         <v>30</v>
@@ -3873,7 +3873,7 @@
         <v>3</v>
       </c>
       <c r="AA21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB21" s="8">
         <v>5</v>
@@ -3882,19 +3882,19 @@
         <v>8</v>
       </c>
       <c r="AD21" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE21" s="8">
         <v>11</v>
       </c>
       <c r="AF21" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG21" s="11" t="s">
         <v>40</v>
       </c>
       <c r="AH21" s="11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="AI21" s="8" t="s">
         <v>3</v>
@@ -3909,7 +3909,7 @@
         <v>91</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>7</v>
@@ -3939,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M22" s="13">
         <v>7</v>
@@ -3954,13 +3954,13 @@
         <v>5</v>
       </c>
       <c r="Q22" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R22" s="13">
         <v>5</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T22" s="13">
         <v>45</v>
@@ -3972,7 +3972,7 @@
         <v>5</v>
       </c>
       <c r="W22" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X22" s="46">
         <v>3.75</v>
@@ -3984,7 +3984,7 @@
         <v>5</v>
       </c>
       <c r="AA22" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB22" s="13">
         <v>5</v>
@@ -4020,7 +4020,7 @@
         <v>92</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>0</v>
@@ -4038,7 +4038,7 @@
         <v>20</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I23" s="8">
         <v>17</v>
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M23" s="8">
         <v>2</v>
@@ -4065,13 +4065,13 @@
         <v>5</v>
       </c>
       <c r="Q23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R23" s="8">
         <v>3</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T23" s="8">
         <v>48</v>
@@ -4083,7 +4083,7 @@
         <v>17</v>
       </c>
       <c r="W23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X23" s="46">
         <v>24</v>
@@ -4095,7 +4095,7 @@
         <v>4</v>
       </c>
       <c r="AA23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB23" s="8">
         <v>5</v>
@@ -4104,25 +4104,25 @@
         <v>17</v>
       </c>
       <c r="AD23" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE23" s="8">
         <v>17</v>
       </c>
       <c r="AF23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG23" s="11" t="s">
         <v>43</v>
       </c>
       <c r="AH23" s="11" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="AI23" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ23" s="11" t="s">
-        <v>133</v>
+        <v>254</v>
       </c>
       <c r="AK23" s="28" t="s">
         <v>121</v>
@@ -4133,7 +4133,7 @@
         <v>93</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>0</v>
@@ -4151,7 +4151,7 @@
         <v>20</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I24" s="13">
         <v>79</v>
@@ -4178,13 +4178,13 @@
         <v>5</v>
       </c>
       <c r="Q24" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R24" s="13">
         <v>5</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T24" s="13">
         <v>45</v>
@@ -4211,7 +4211,7 @@
         <v>3</v>
       </c>
       <c r="AB24" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC24" s="13">
         <v>24</v>
@@ -4229,7 +4229,7 @@
         <v>119</v>
       </c>
       <c r="AH24" s="17" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="AI24" s="13" t="s">
         <v>3</v>
@@ -4244,7 +4244,7 @@
         <v>94</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>7</v>
@@ -4274,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M25" s="8">
         <v>3</v>
@@ -4289,7 +4289,7 @@
         <v>3</v>
       </c>
       <c r="Q25" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R25" s="8">
         <v>5</v>
@@ -4319,7 +4319,7 @@
         <v>2</v>
       </c>
       <c r="AA25" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB25" s="8">
         <v>5</v>
@@ -4328,13 +4328,13 @@
         <v>7</v>
       </c>
       <c r="AD25" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE25" s="8">
         <v>7</v>
       </c>
       <c r="AF25" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG25" s="11" t="s">
         <v>45</v>
@@ -4343,7 +4343,7 @@
         <v>46</v>
       </c>
       <c r="AI25" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ25" s="11" t="s">
         <v>47</v>
@@ -4357,7 +4357,7 @@
         <v>95</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>7</v>
@@ -4402,13 +4402,13 @@
         <v>5</v>
       </c>
       <c r="Q26" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R26" s="13">
         <v>5</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T26" s="13">
         <v>47.5</v>
@@ -4420,7 +4420,7 @@
         <v>14</v>
       </c>
       <c r="W26" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X26" s="46">
         <v>5</v>
@@ -4432,7 +4432,7 @@
         <v>2</v>
       </c>
       <c r="AA26" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB26" s="13">
         <v>4</v>
@@ -4453,7 +4453,7 @@
         <v>121</v>
       </c>
       <c r="AH26" s="17" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="AI26" s="13" t="s">
         <v>3</v>
@@ -4468,7 +4468,7 @@
         <v>96</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>7</v>
@@ -4498,7 +4498,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M27" s="8">
         <v>3</v>
@@ -4513,13 +4513,13 @@
         <v>5</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R27" s="8">
         <v>4</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T27" s="8">
         <v>45</v>
@@ -4543,7 +4543,7 @@
         <v>2</v>
       </c>
       <c r="AA27" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB27" s="8">
         <v>5</v>
@@ -4552,7 +4552,7 @@
         <v>5</v>
       </c>
       <c r="AD27" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE27" s="8">
         <v>5</v>
@@ -4579,7 +4579,7 @@
         <v>97</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>0</v>
@@ -4597,7 +4597,7 @@
         <v>20</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="I28" s="13">
         <v>8</v>
@@ -4609,7 +4609,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M28" s="13">
         <v>3</v>
@@ -4630,7 +4630,7 @@
         <v>2</v>
       </c>
       <c r="S28" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T28" s="13">
         <v>40</v>
@@ -4654,7 +4654,7 @@
         <v>2</v>
       </c>
       <c r="AA28" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB28" s="13">
         <v>2</v>
@@ -4663,28 +4663,28 @@
         <v>8</v>
       </c>
       <c r="AD28" s="14" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE28" s="13">
         <v>8</v>
       </c>
       <c r="AF28" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG28" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH28" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI28" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ28" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="AK28" s="30" t="s">
         <v>169</v>
-      </c>
-      <c r="AH28" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI28" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ28" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="AK28" s="30" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
@@ -4692,7 +4692,7 @@
         <v>98</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>7</v>
@@ -4722,7 +4722,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M29" s="8">
         <v>2</v>
@@ -4743,7 +4743,7 @@
         <v>3</v>
       </c>
       <c r="S29" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T29" s="8">
         <v>40</v>
@@ -4767,7 +4767,7 @@
         <v>1.5</v>
       </c>
       <c r="AA29" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB29" s="8">
         <v>4</v>
@@ -4776,7 +4776,7 @@
         <v>18</v>
       </c>
       <c r="AD29" s="8" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE29" s="8">
         <v>18</v>
@@ -4791,7 +4791,7 @@
         <v>126</v>
       </c>
       <c r="AI29" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ29" s="11" t="s">
         <v>52</v>
@@ -4805,7 +4805,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>7</v>
@@ -4829,13 +4829,13 @@
         <v>77</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K30" s="14">
         <v>3</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M30" s="13">
         <v>4</v>
@@ -4856,7 +4856,7 @@
         <v>3</v>
       </c>
       <c r="S30" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T30" s="13">
         <v>49</v>
@@ -4880,7 +4880,7 @@
         <v>0.67</v>
       </c>
       <c r="AA30" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB30" s="13">
         <v>4</v>
@@ -4916,7 +4916,7 @@
         <v>100</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>7</v>
@@ -4946,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M31" s="8">
         <v>2</v>
@@ -4961,7 +4961,7 @@
         <v>3</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R31" s="8">
         <v>3</v>
@@ -4991,7 +4991,7 @@
         <v>4</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB31" s="8">
         <v>3</v>
@@ -5012,16 +5012,16 @@
         <v>121</v>
       </c>
       <c r="AH31" s="11" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="AI31" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ31" s="11" t="s">
-        <v>172</v>
+        <v>245</v>
       </c>
       <c r="AK31" s="12" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
@@ -5029,7 +5029,7 @@
         <v>101</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>7</v>
@@ -5059,7 +5059,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M32" s="13">
         <v>3</v>
@@ -5074,13 +5074,13 @@
         <v>4</v>
       </c>
       <c r="Q32" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R32" s="13">
         <v>4</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T32" s="13">
         <v>47.5</v>
@@ -5104,7 +5104,7 @@
         <v>4</v>
       </c>
       <c r="AA32" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB32" s="13">
         <v>4</v>
@@ -5113,19 +5113,19 @@
         <v>6</v>
       </c>
       <c r="AD32" s="43" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE32" s="13">
         <v>6</v>
       </c>
       <c r="AF32" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG32" s="27" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="AH32" s="17" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="AI32" s="13" t="s">
         <v>3</v>
@@ -5140,7 +5140,7 @@
         <v>102</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>7</v>
@@ -5164,13 +5164,13 @@
         <v>238</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K33" s="8">
         <v>4</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M33" s="8">
         <v>2</v>
@@ -5218,13 +5218,13 @@
         <v>3</v>
       </c>
       <c r="AB33" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC33" s="8">
         <v>166</v>
       </c>
       <c r="AD33" s="47" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE33" s="8">
         <v>48</v>
@@ -5236,16 +5236,16 @@
         <v>121</v>
       </c>
       <c r="AH33" s="11" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="AI33" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ33" s="11" t="s">
-        <v>175</v>
+        <v>246</v>
       </c>
       <c r="AK33" s="12" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
@@ -5253,7 +5253,7 @@
         <v>103</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>0</v>
@@ -5271,19 +5271,19 @@
         <v>48</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I34" s="13">
         <v>24</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K34" s="13">
         <v>3</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M34" s="13">
         <v>4</v>
@@ -5304,7 +5304,7 @@
         <v>3</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T34" s="13">
         <v>45</v>
@@ -5328,7 +5328,7 @@
         <v>1.5</v>
       </c>
       <c r="AA34" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB34" s="14">
         <v>4</v>
@@ -5337,25 +5337,25 @@
         <v>12</v>
       </c>
       <c r="AD34" s="14" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE34" s="13">
         <v>24</v>
       </c>
       <c r="AF34" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG34" s="27" t="s">
         <v>120</v>
       </c>
       <c r="AH34" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AI34" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ34" s="17" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="AK34" s="20" t="s">
         <v>121</v>
@@ -5366,7 +5366,7 @@
         <v>104</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>0</v>
@@ -5384,19 +5384,19 @@
         <v>48</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="I35" s="8">
         <v>25</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K35" s="8">
         <v>2</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M35" s="8">
         <v>2</v>
@@ -5417,7 +5417,7 @@
         <v>3</v>
       </c>
       <c r="S35" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T35" s="8">
         <v>40</v>
@@ -5429,7 +5429,7 @@
         <v>17</v>
       </c>
       <c r="W35" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X35" s="46">
         <v>20</v>
@@ -5441,7 +5441,7 @@
         <v>1.5</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB35" s="8">
         <v>3</v>
@@ -5456,10 +5456,10 @@
         <v>8</v>
       </c>
       <c r="AF35" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG35" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AH35" s="11" t="s">
         <v>58</v>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:37" ht="118.8" x14ac:dyDescent="0.25">
@@ -5477,13 +5477,13 @@
         <v>105</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>2</v>
@@ -5501,13 +5501,13 @@
         <v>103</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K36" s="13">
         <v>2</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M36" s="13">
         <v>3</v>
@@ -5528,7 +5528,7 @@
         <v>5</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T36" s="13">
         <v>40</v>
@@ -5552,7 +5552,7 @@
         <v>1.5</v>
       </c>
       <c r="AA36" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB36" s="13">
         <v>5</v>
@@ -5567,22 +5567,22 @@
         <v>70</v>
       </c>
       <c r="AF36" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG36" s="17" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="AH36" s="17" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="AI36" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ36" s="27" t="s">
         <v>59</v>
       </c>
       <c r="AK36" s="18" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
@@ -5590,7 +5590,7 @@
         <v>106</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>0</v>
@@ -5620,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M37" s="8">
         <v>1</v>
@@ -5635,7 +5635,7 @@
         <v>5</v>
       </c>
       <c r="Q37" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R37" s="8">
         <v>5</v>
@@ -5665,7 +5665,7 @@
         <v>2.25</v>
       </c>
       <c r="AA37" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB37" s="8">
         <v>5</v>
@@ -5686,10 +5686,10 @@
         <v>121</v>
       </c>
       <c r="AH37" s="11" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="AI37" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ37" s="11" t="s">
         <v>39</v>
@@ -5703,7 +5703,7 @@
         <v>107</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>7</v>
@@ -5748,13 +5748,13 @@
         <v>3</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R38" s="13">
         <v>4</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T38" s="13">
         <v>42.5</v>
@@ -5766,7 +5766,7 @@
         <v>14</v>
       </c>
       <c r="W38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X38" s="46">
         <v>10</v>
@@ -5778,7 +5778,7 @@
         <v>1.5</v>
       </c>
       <c r="AA38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB38" s="13">
         <v>3</v>
@@ -5787,28 +5787,28 @@
         <v>30</v>
       </c>
       <c r="AD38" s="13" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE38" s="13">
         <v>30</v>
       </c>
       <c r="AF38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG38" s="27" t="s">
         <v>60</v>
       </c>
       <c r="AH38" s="17" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="AI38" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ38" s="17" t="s">
-        <v>179</v>
+        <v>247</v>
       </c>
       <c r="AK38" s="30" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
@@ -5816,13 +5816,13 @@
         <v>108</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>131</v>
@@ -5846,7 +5846,7 @@
         <v>1</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M39" s="8">
         <v>3</v>
@@ -5894,7 +5894,7 @@
         <v>3</v>
       </c>
       <c r="AB39" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC39" s="8">
         <v>96</v>
@@ -5912,7 +5912,7 @@
         <v>121</v>
       </c>
       <c r="AH39" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AI39" s="8" t="s">
         <v>3</v>
@@ -5927,7 +5927,7 @@
         <v>109</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>7</v>
@@ -5951,7 +5951,7 @@
         <v>21</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K40" s="14">
         <v>2</v>
@@ -5978,7 +5978,7 @@
         <v>2</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T40" s="13">
         <v>55</v>
@@ -5990,7 +5990,7 @@
         <v>14</v>
       </c>
       <c r="W40" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="X40" s="46">
         <v>30</v>
@@ -6005,7 +6005,7 @@
         <v>3</v>
       </c>
       <c r="AB40" s="44" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AC40" s="13">
         <v>8</v>
@@ -6017,22 +6017,22 @@
         <v>8</v>
       </c>
       <c r="AF40" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG40" s="27" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="AH40" s="17" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="AI40" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ40" s="27" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="AK40" s="30" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:37" ht="66" x14ac:dyDescent="0.25">
@@ -6040,7 +6040,7 @@
         <v>110</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>0</v>
@@ -6115,7 +6115,7 @@
         <v>0</v>
       </c>
       <c r="AA41" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB41" s="8">
         <v>3</v>
@@ -6139,10 +6139,10 @@
         <v>65</v>
       </c>
       <c r="AI41" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AJ41" s="11" t="s">
-        <v>183</v>
+        <v>249</v>
       </c>
       <c r="AK41" s="28" t="s">
         <v>121</v>
@@ -6153,7 +6153,7 @@
         <v>111</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C42" s="32" t="s">
         <v>0</v>
@@ -6183,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M42" s="32">
         <v>3</v>
@@ -6204,7 +6204,7 @@
         <v>4</v>
       </c>
       <c r="S42" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T42" s="32">
         <v>25</v>
@@ -6228,7 +6228,7 @@
         <v>4</v>
       </c>
       <c r="AA42" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AB42" s="32">
         <v>3</v>
@@ -6237,7 +6237,7 @@
         <v>4</v>
       </c>
       <c r="AD42" s="48" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="AE42" s="34">
         <v>4</v>

</xml_diff>

<commit_message>
Se termina el EDA y se añade tabla sobre abandono de empleados en 2024
</commit_message>
<xml_diff>
--- a/data/raw/survey_ready.xlsx
+++ b/data/raw/survey_ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAA0600-CA9F-4563-8866-D0BC9829F7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6503BBE7-95A3-490D-915E-EEC6FA6D2141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2294,7 +2294,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1A3DD08-FFAC-45FE-BDA2-A5F8F5F0C34A}" name="Tabla1" displayName="Tabla1" ref="A1:AK42" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="A1:AK42" xr:uid="{C1A3DD08-FFAC-45FE-BDA2-A5F8F5F0C34A}"/>
+  <autoFilter ref="A1:AK42" xr:uid="{C1A3DD08-FFAC-45FE-BDA2-A5F8F5F0C34A}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Divorciado/a"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{A696CABF-A4D0-4A9D-8A88-58BFB363F0A0}" name="id_empleado" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{F2CBB998-2073-4685-BB3C-614B54051001}" name="rango_edad" dataDxfId="25"/>
@@ -2541,7 +2547,7 @@
   </sheetPr>
   <dimension ref="A1:AK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AK2" sqref="AK2"/>
     </sheetView>
@@ -2701,7 +2707,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="158.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="158.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>68</v>
       </c>
@@ -3036,7 +3042,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>70</v>
       </c>
@@ -3260,7 +3266,7 @@
       </c>
       <c r="AK6" s="18"/>
     </row>
-    <row r="7" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -3371,7 +3377,7 @@
       </c>
       <c r="AK7" s="19"/>
     </row>
-    <row r="8" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>72</v>
       </c>
@@ -3480,7 +3486,7 @@
       </c>
       <c r="AK8" s="21"/>
     </row>
-    <row r="9" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>73</v>
       </c>
@@ -3593,7 +3599,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>74</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" ht="92.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>75</v>
       </c>
@@ -3817,7 +3823,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>76</v>
       </c>
@@ -3928,7 +3934,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>77</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>78</v>
       </c>
@@ -4152,7 +4158,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>79</v>
       </c>
@@ -4263,7 +4269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="184.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>80</v>
       </c>
@@ -4376,7 +4382,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>81</v>
       </c>
@@ -4485,7 +4491,7 @@
       </c>
       <c r="AK17" s="24"/>
     </row>
-    <row r="18" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>82</v>
       </c>
@@ -4594,7 +4600,7 @@
       </c>
       <c r="AK18" s="20"/>
     </row>
-    <row r="19" spans="1:37" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" ht="92.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>83</v>
       </c>
@@ -4705,7 +4711,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" ht="145.19999999999999" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>84</v>
       </c>
@@ -4818,7 +4824,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>85</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>86</v>
       </c>
@@ -5042,7 +5048,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -5151,7 +5157,7 @@
       </c>
       <c r="AK23" s="24"/>
     </row>
-    <row r="24" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>88</v>
       </c>
@@ -5264,7 +5270,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -5373,7 +5379,7 @@
       </c>
       <c r="AK25" s="24"/>
     </row>
-    <row r="26" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>90</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>91</v>
       </c>
@@ -5595,7 +5601,7 @@
       </c>
       <c r="AK27" s="27"/>
     </row>
-    <row r="28" spans="1:37" ht="198" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" ht="198" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>92</v>
       </c>
@@ -5706,7 +5712,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>93</v>
       </c>
@@ -5815,7 +5821,7 @@
       </c>
       <c r="AK29" s="24"/>
     </row>
-    <row r="30" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>94</v>
       </c>
@@ -5926,7 +5932,7 @@
       </c>
       <c r="AK30" s="21"/>
     </row>
-    <row r="31" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>95</v>
       </c>
@@ -6039,7 +6045,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" ht="26.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>96</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>98</v>
       </c>
@@ -6370,7 +6376,7 @@
       </c>
       <c r="AK34" s="17"/>
     </row>
-    <row r="35" spans="1:37" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" ht="79.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>99</v>
       </c>
@@ -6483,7 +6489,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" ht="118.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>100</v>
       </c>
@@ -6596,7 +6602,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" ht="39.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>101</v>
       </c>
@@ -6707,7 +6713,7 @@
       </c>
       <c r="AK37" s="24"/>
     </row>
-    <row r="38" spans="1:37" ht="66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" ht="66" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -6818,7 +6824,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>103</v>
       </c>
@@ -6929,7 +6935,7 @@
       </c>
       <c r="AK39" s="27"/>
     </row>
-    <row r="40" spans="1:37" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" ht="105.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>104</v>
       </c>
@@ -7042,7 +7048,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" ht="52.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>105</v>
       </c>
@@ -7153,7 +7159,7 @@
       </c>
       <c r="AK41" s="24"/>
     </row>
-    <row r="42" spans="1:37" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>106</v>
       </c>

</xml_diff>